<commit_message>
Nasar - 09Nov changes
</commit_message>
<xml_diff>
--- a/src/test/resources/object-repository/OneCSApp.xlsx
+++ b/src/test/resources/object-repository/OneCSApp.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10411"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA3B5935-2054-394B-8C0B-11B15474E50D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945C301F-6A96-EA4A-AFAE-DD35F0B017AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="164">
   <si>
     <t>ELEMENT_KEY</t>
   </si>
@@ -490,6 +490,30 @@
   </si>
   <si>
     <t>//android.widget.TextView[@text='Reports']</t>
+  </si>
+  <si>
+    <t>PORTFOLIO_SHOWALL_DOWN_ARROW</t>
+  </si>
+  <si>
+    <t>ic_expand_pill</t>
+  </si>
+  <si>
+    <t>portfolio-performance-increase-arrow</t>
+  </si>
+  <si>
+    <t>PORTFOLIO_PERFORMANCE_ARROW</t>
+  </si>
+  <si>
+    <t>portfolio-summary-value-change</t>
+  </si>
+  <si>
+    <t>PORTFOLIO_SUMMARY_VALUE_CHANGE_TXT</t>
+  </si>
+  <si>
+    <t>portfolio-summary-refreshed-at-text</t>
+  </si>
+  <si>
+    <t>PORTFOLIO_SUMMARY_REFRESH_TIME_TXT</t>
   </si>
 </sst>
 </file>
@@ -864,10 +888,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1206,10 +1230,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>157</v>
       </c>
       <c r="E30" t="s">
         <v>25</v>
@@ -1271,7 +1295,40 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>159</v>
+      </c>
+      <c r="B36" t="s">
+        <v>158</v>
+      </c>
       <c r="E36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>161</v>
+      </c>
+      <c r="B37" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>163</v>
+      </c>
+      <c r="B38" t="s">
+        <v>162</v>
+      </c>
+      <c r="E38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>